<commit_message>
added graphs for each pair of experiments
</commit_message>
<xml_diff>
--- a/experiments/2014-01-04/Combined-A-through-D.xlsx
+++ b/experiments/2014-01-04/Combined-A-through-D.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="40" windowWidth="30360" windowHeight="20260" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="0" windowWidth="30360" windowHeight="20260" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="3" r:id="rId1"/>
@@ -166,8 +166,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -209,7 +213,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -224,6 +228,8 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -238,6 +244,8 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -246,6 +254,988 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Experiment 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>A1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'A1'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'A1'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>55.39419661416547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.82500622801963</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.779342242439048</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>A2'</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'A2'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>54.6480999314535</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38.03814934124161</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.51768924586763</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.619663699001516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="541274280"/>
+        <c:axId val="539700984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="541274280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from the Raspberry Pi</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539700984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="539700984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Times Seen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="541274280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Experiment B</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>B1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'B1'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'B1'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>55.36208170186872</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.40333027633025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.06920420360862</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>B2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'B2'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>53.99471124750767</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.00341991233595</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.51155696574682</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="538160008"/>
+        <c:axId val="542871848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="538160008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from the Raspberry</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Pi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="542871848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="542871848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Times Seen</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="538160008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Experiment C</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="1"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>C1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'C1'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'C1'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>54.91924074616914</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.96460357428748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.755235074159449</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.988530913495015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>C2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'C2'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>54.68501572855828</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.22262863898062</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.295312851177188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="543139672"/>
+        <c:axId val="580017304"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="543139672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from the Raspberry</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Pi</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="580017304"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="580017304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Times Seen (per sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="543139672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Exercise D</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>D1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D1'!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'D1'!$I$2:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>54.67214704374206</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.09798417400587</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.669316581882128</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="539498760"/>
+        <c:axId val="539364152"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="539498760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from the Raspberry Pi</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539364152"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="539364152"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Times Seen (per sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="539498760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
@@ -620,11 +1610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="442183960"/>
-        <c:axId val="442394216"/>
+        <c:axId val="499030856"/>
+        <c:axId val="499033832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="442183960"/>
+        <c:axId val="499030856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -633,7 +1623,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442394216"/>
+        <c:crossAx val="499033832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -641,7 +1631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="442394216"/>
+        <c:axId val="499033832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -652,13 +1642,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="442183960"/>
+        <c:crossAx val="499030856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -673,7 +1664,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
@@ -922,11 +1913,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="441866392"/>
-        <c:axId val="441869448"/>
+        <c:axId val="520099048"/>
+        <c:axId val="520102104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="441866392"/>
+        <c:axId val="520099048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -935,7 +1926,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441869448"/>
+        <c:crossAx val="520102104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -943,7 +1934,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="441869448"/>
+        <c:axId val="520102104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,14 +1945,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="441866392"/>
+        <c:crossAx val="520099048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -977,6 +1967,146 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1295400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1013,7 +2143,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1372,8 +2502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1611,6 +2741,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1898,7 +3029,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2122,6 +3253,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2370,7 +3502,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2616,6 +3748,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2934,7 +4067,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3203,6 +4336,7 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3215,7 +4349,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Combined all related experiments and added graphs
</commit_message>
<xml_diff>
--- a/experiments/2014-01-04/Combined-A-through-D.xlsx
+++ b/experiments/2014-01-04/Combined-A-through-D.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="0" windowWidth="30360" windowHeight="20260" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="6440" yWindow="0" windowWidth="30360" windowHeight="20260" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="3" r:id="rId1"/>
@@ -14,8 +14,9 @@
     <sheet name="C1" sheetId="1" r:id="rId5"/>
     <sheet name="C2" sheetId="2" r:id="rId6"/>
     <sheet name="D1" sheetId="5" r:id="rId7"/>
-    <sheet name="Absolute graph" sheetId="8" r:id="rId8"/>
-    <sheet name="Relative graph" sheetId="9" r:id="rId9"/>
+    <sheet name="D2" sheetId="10" r:id="rId8"/>
+    <sheet name="Absolute graph" sheetId="8" r:id="rId9"/>
+    <sheet name="Relative graph" sheetId="9" r:id="rId10"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="34">
   <si>
     <t>0ft</t>
   </si>
@@ -100,6 +101,36 @@
   <si>
     <t>Transmissions per sec</t>
   </si>
+  <si>
+    <t>Experiment name</t>
+  </si>
+  <si>
+    <t>Experiment number</t>
+  </si>
+  <si>
+    <t>Device address</t>
+  </si>
+  <si>
+    <t>Device name</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>First timestamp</t>
+  </si>
+  <si>
+    <t>Second timestamp</t>
+  </si>
+  <si>
+    <t>51:FC:6C:5D:13:B4</t>
+  </si>
+  <si>
+    <t>35ft</t>
+  </si>
+  <si>
+    <t>A1-D2</t>
+  </si>
 </sst>
 </file>
 
@@ -166,8 +197,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -213,7 +250,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -230,6 +267,9 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -246,6 +286,9 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,11 +456,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="541274280"/>
-        <c:axId val="539700984"/>
+        <c:axId val="424303272"/>
+        <c:axId val="424310168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="541274280"/>
+        <c:axId val="424303272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539700984"/>
+        <c:crossAx val="424310168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -453,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539700984"/>
+        <c:axId val="424310168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -483,7 +526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="541274280"/>
+        <c:crossAx val="424303272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -665,11 +708,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="538160008"/>
-        <c:axId val="542871848"/>
+        <c:axId val="422964584"/>
+        <c:axId val="422970344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="538160008"/>
+        <c:axId val="422964584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -702,7 +745,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="542871848"/>
+        <c:crossAx val="422970344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -710,7 +753,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="542871848"/>
+        <c:axId val="422970344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -740,7 +783,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="538160008"/>
+        <c:crossAx val="422964584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,11 +965,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="543139672"/>
-        <c:axId val="580017304"/>
+        <c:axId val="423018056"/>
+        <c:axId val="423023816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="543139672"/>
+        <c:axId val="423018056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +1002,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="580017304"/>
+        <c:crossAx val="423023816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -967,7 +1010,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="580017304"/>
+        <c:axId val="423023816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1002,7 +1045,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="543139672"/>
+        <c:crossAx val="423018056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1055,7 +1098,7 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1133,6 +1176,50 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>D2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'D2'!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>53.54705085263797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.3471438960699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.86089865416316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.573290225419121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1143,11 +1230,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="539498760"/>
-        <c:axId val="539364152"/>
+        <c:axId val="424373064"/>
+        <c:axId val="424378616"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="539498760"/>
+        <c:axId val="424373064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1175,7 +1262,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539364152"/>
+        <c:crossAx val="424378616"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1183,7 +1270,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="539364152"/>
+        <c:axId val="424378616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1213,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="539498760"/>
+        <c:crossAx val="424373064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1600,6 +1687,50 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:v>D2</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'D2'!$I$2:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>53.54705085263797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34.3471438960699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.86089865416316</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.573290225419121</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1610,11 +1741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="499030856"/>
-        <c:axId val="499033832"/>
+        <c:axId val="424435256"/>
+        <c:axId val="424438232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="499030856"/>
+        <c:axId val="424435256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1623,7 +1754,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499033832"/>
+        <c:crossAx val="424438232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1631,7 +1762,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="499033832"/>
+        <c:axId val="424438232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1773,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="499030856"/>
+        <c:crossAx val="424435256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1694,9 +1825,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'B1'!$A$2:$A$8</c:f>
+              <c:f>'D2'!$A$2:$A$9</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0ft</c:v>
                 </c:pt>
@@ -1717,6 +1848,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1759,6 +1893,38 @@
             <c:v>A1-B2</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'B2'!$K$2:$K$8</c:f>
@@ -1797,6 +1963,38 @@
             <c:v>A1-C1</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'C1'!$K$2:$K$8</c:f>
@@ -1835,6 +2033,38 @@
             <c:v>A1-C2</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'C2'!$K$2:$K$8</c:f>
@@ -1873,6 +2103,38 @@
             <c:v>A1-D1</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'D1'!$K$2:$K$8</c:f>
@@ -1899,6 +2161,79 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>A1-D2</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'D2'!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0ft</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5ft</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10ft</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15ft</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20ft</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25ft</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30ft</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35ft</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'D2'!$K$2:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.8471457615275</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.47786233194973</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.560898654163157</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-7.793947982980073</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1913,11 +2248,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="520099048"/>
-        <c:axId val="520102104"/>
+        <c:axId val="424478200"/>
+        <c:axId val="424481256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="520099048"/>
+        <c:axId val="424478200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1926,7 +2261,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520102104"/>
+        <c:crossAx val="424481256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1934,7 +2269,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="520102104"/>
+        <c:axId val="424481256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1945,13 +2280,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520099048"/>
+        <c:crossAx val="424478200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2075,16 +2411,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>952500</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2750,6 +3086,24 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I8"/>
@@ -4066,8 +4420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4347,9 +4701,344 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="3" width="18.1640625" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>606</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1389735811.9816401</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1389735823.29879</v>
+      </c>
+      <c r="H2" s="1">
+        <f>G2-F2</f>
+        <v>11.317149877548218</v>
+      </c>
+      <c r="I2">
+        <f>E2/MAX(H2,10)</f>
+        <v>53.547050852637973</v>
+      </c>
+      <c r="K2">
+        <f>'A1'!I2-'D2'!I2</f>
+        <v>1.8471457615275</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>422</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1389735863.2959399</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1389735875.5822599</v>
+      </c>
+      <c r="H3" s="1">
+        <f t="shared" ref="H3:H9" si="0">G3-F3</f>
+        <v>12.286319971084595</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I9" si="1">E3/MAX(H3,10)</f>
+        <v>34.347143896069902</v>
+      </c>
+      <c r="K3">
+        <f>'A1'!I3-'D2'!I3</f>
+        <v>4.4778623319497299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>154</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1389735906.8274901</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1389735918.80177</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" si="0"/>
+        <v>11.974279880523682</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>12.860898654163158</v>
+      </c>
+      <c r="K4">
+        <f>'A1'!I4-'D2'!I4</f>
+        <v>-4.5608986541631573</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>105</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1389735940.82303</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1389735953.07037</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="0"/>
+        <v>12.247339963912964</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>8.5732902254191217</v>
+      </c>
+      <c r="K5">
+        <f>'A1'!I5-'D2'!I5</f>
+        <v>-7.7939479829800735</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>36</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1389735978.1619401</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1389735987.66593</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="0"/>
+        <v>9.5039899349212646</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+      <c r="K6">
+        <f>'A1'!I6-'D2'!I6</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1389736014.0503199</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1389736020.8054299</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7551100254058838</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="K7">
+        <f>'A1'!I7-'D2'!I7</f>
+        <v>-2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1389736052.39469</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1389736055.6700301</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2753400802612305</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="K8">
+        <f>'A1'!I8-'D2'!I8</f>
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1389736094.2030699</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1389736094.3951199</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19204998016357422</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="K9">
+        <f>'A1'!I9-'D2'!I9</f>
+        <v>-0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -4363,22 +5052,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>